<commit_message>
demo dataset for the NoiseCompressor project
</commit_message>
<xml_diff>
--- a/noise_compressor/demo_dataset/stem_information.xlsx
+++ b/noise_compressor/demo_dataset/stem_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uqoca.sharepoint.com/sites/MEC-PN-PR/Documents partages/General/article_compression/projetPython/NoiseCompressorQt/demo_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\PycharmProjects\Sample_Data\noise_compressor\demo_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{60FDF49B-7E14-47C7-B5FB-AF8D25E6B07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B0BB0D1-1F80-453A-9EEA-8B656FAE0911}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B858673-3139-4A21-ADCD-5BFFBB85BD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE1FD152-1768-4D12-AC71-A38632524EE4}"/>
   </bookViews>
@@ -37,7 +37,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+  <si>
+    <t>10001.ply</t>
+  </si>
+  <si>
+    <t>10002.ply</t>
+  </si>
+  <si>
+    <t>10004.ply</t>
+  </si>
+  <si>
+    <t>10006.ply</t>
+  </si>
+  <si>
+    <t>10008.ply</t>
+  </si>
+  <si>
+    <t>10010.ply</t>
+  </si>
+  <si>
+    <t>10809.ply</t>
+  </si>
+  <si>
+    <t>11011.ply</t>
+  </si>
+  <si>
+    <t>11315.ply</t>
+  </si>
+  <si>
+    <t>11820.ply</t>
+  </si>
+  <si>
+    <t>12323.ply</t>
+  </si>
+  <si>
+    <t>12628.ply</t>
+  </si>
+  <si>
+    <t>13031.ply</t>
+  </si>
+  <si>
+    <t>13335.ply</t>
+  </si>
+  <si>
+    <t>13638.ply</t>
+  </si>
+  <si>
+    <t>14445.ply</t>
+  </si>
+  <si>
+    <t>14648.ply</t>
+  </si>
   <si>
     <t>stem_id</t>
   </si>
@@ -69,10 +120,43 @@
     <t>Actual stem diameter measurement  (in meter) at breast height</t>
   </si>
   <si>
+    <t>20506.ply</t>
+  </si>
+  <si>
+    <t>20607.ply</t>
+  </si>
+  <si>
     <t>20709.ply</t>
   </si>
   <si>
+    <t>20809.ply</t>
+  </si>
+  <si>
+    <t>21112.ply</t>
+  </si>
+  <si>
+    <t>21315.ply</t>
+  </si>
+  <si>
+    <t>21617.ply</t>
+  </si>
+  <si>
+    <t>21719.ply</t>
+  </si>
+  <si>
+    <t>22526.ply</t>
+  </si>
+  <si>
     <t>22729.ply</t>
+  </si>
+  <si>
+    <t>22830.ply</t>
+  </si>
+  <si>
+    <t>23132.ply</t>
+  </si>
+  <si>
+    <t>23436.ply</t>
   </si>
 </sst>
 </file>
@@ -497,42 +581,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -542,10 +626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154DEEC-CC39-4E66-B85F-F2BBD06A6C32}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,43 +639,435 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>10001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2">
+        <v>1.01E-2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>10002</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>10004</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10006</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="C5" s="2">
+        <v>6.5700000000000008E-2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>10008</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>10010</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>10809</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>11011</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.105</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>11315</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>11820</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12323</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12628</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13031</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13335</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>13638</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>14445</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>14648</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>20506</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>20607</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <v>20709</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2">
         <v>0.08</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>20809</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>21112</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>21315</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>21617</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>21719</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>22526</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.255</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <v>22729</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>22830</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>23132</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.315</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>23436</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
     </row>

</xml_diff>